<commit_message>
Add PHY2033 to 3rd year options, make stats 4th year prereqs compulsory for GGC3
</commit_message>
<xml_diff>
--- a/Modules.xlsx
+++ b/Modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joematthews/Desktop/PreReg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7423792B-EE5F-3041-B36B-F76AF4A80615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9960C115-F77D-AB49-88C6-07DF664F52BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Working App back end " sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Working App back end '!$A$1:$K$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Working App back end '!$A$1:$K$125</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="381">
   <si>
     <t>Code</t>
   </si>
@@ -721,9 +721,6 @@
     <t>PHY3029</t>
   </si>
   <si>
-    <t>PHY3029 Variational Methods&amp;Langrangian Dynamics</t>
-  </si>
-  <si>
     <t>PHY3032</t>
   </si>
   <si>
@@ -1141,15 +1138,9 @@
     <t>PHY2036 Thermodynamics &amp; Statistical Mechanics</t>
   </si>
   <si>
-    <t>F300;F303;F3FM;f344</t>
-  </si>
-  <si>
     <t>F3F5;F3FM;F303;F344;F345</t>
   </si>
   <si>
-    <t>F3F5;F3FM;F344;FS45</t>
-  </si>
-  <si>
     <t>F344;F3FM</t>
   </si>
   <si>
@@ -1175,6 +1166,21 @@
   </si>
   <si>
     <t>F303;MPWA2</t>
+  </si>
+  <si>
+    <t>GGC3</t>
+  </si>
+  <si>
+    <t>PHY2033 Fluid Dynamics (Stage 3)</t>
+  </si>
+  <si>
+    <t>PHY3029 Variational Methods &amp;Langrangian Dynamics</t>
+  </si>
+  <si>
+    <t>F300;F303;F3FM;F344</t>
+  </si>
+  <si>
+    <t>F3F5;F3FM;F344;F345</t>
   </si>
 </sst>
 </file>
@@ -2057,13 +2063,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O124"/>
+  <dimension ref="A1:O125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H98" sqref="H98"/>
+      <selection pane="bottomRight" activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2118,16 +2124,16 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="O1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -2153,7 +2159,7 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -2200,7 +2206,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -2215,7 +2221,7 @@
         <v>37</v>
       </c>
       <c r="M3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N3" t="s">
         <v>37</v>
@@ -2247,7 +2253,7 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
@@ -2294,7 +2300,7 @@
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -2341,7 +2347,7 @@
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
@@ -2388,7 +2394,7 @@
         <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
@@ -2435,7 +2441,7 @@
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
@@ -2482,7 +2488,7 @@
         <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
@@ -2529,7 +2535,7 @@
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -2576,7 +2582,7 @@
         <v>23</v>
       </c>
       <c r="H11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I11" t="s">
         <v>17</v>
@@ -2623,7 +2629,7 @@
         <v>23</v>
       </c>
       <c r="H12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
@@ -2670,13 +2676,13 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
       </c>
       <c r="J13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K13" t="s">
         <v>37</v>
@@ -2717,7 +2723,7 @@
         <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I14" t="s">
         <v>17</v>
@@ -2776,7 +2782,7 @@
         <v>62</v>
       </c>
       <c r="L15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M15" t="s">
         <v>61</v>
@@ -2917,7 +2923,7 @@
         <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M18" t="s">
         <v>61</v>
@@ -3058,7 +3064,7 @@
         <v>37</v>
       </c>
       <c r="L21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M21" t="s">
         <v>61</v>
@@ -3199,7 +3205,7 @@
         <v>86</v>
       </c>
       <c r="L24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M24" t="s">
         <v>85</v>
@@ -3340,7 +3346,7 @@
         <v>37</v>
       </c>
       <c r="L27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M27" t="s">
         <v>85</v>
@@ -3434,13 +3440,13 @@
         <v>37</v>
       </c>
       <c r="L29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N29" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O29" t="s">
         <v>37</v>
@@ -3563,7 +3569,7 @@
         <v>23</v>
       </c>
       <c r="H32" t="s">
-        <v>37</v>
+        <v>376</v>
       </c>
       <c r="I32" t="s">
         <v>17</v>
@@ -3716,7 +3722,7 @@
         <v>37</v>
       </c>
       <c r="L35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="M35" t="s">
         <v>115</v>
@@ -3810,7 +3816,7 @@
         <v>37</v>
       </c>
       <c r="L37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M37" t="s">
         <v>115</v>
@@ -3845,7 +3851,7 @@
         <v>15</v>
       </c>
       <c r="H38" t="s">
-        <v>37</v>
+        <v>376</v>
       </c>
       <c r="I38" t="s">
         <v>17</v>
@@ -3904,7 +3910,7 @@
         <v>37</v>
       </c>
       <c r="L39" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M39" t="s">
         <v>110</v>
@@ -3939,7 +3945,7 @@
         <v>57</v>
       </c>
       <c r="H40" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="I40" t="s">
         <v>17</v>
@@ -4236,7 +4242,7 @@
         <v>37</v>
       </c>
       <c r="M46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N46" t="s">
         <v>37</v>
@@ -4430,7 +4436,7 @@
         <v>37</v>
       </c>
       <c r="O50" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -4471,13 +4477,13 @@
         <v>37</v>
       </c>
       <c r="M51" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N51" t="s">
         <v>37</v>
       </c>
       <c r="O51" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -4524,7 +4530,7 @@
         <v>37</v>
       </c>
       <c r="O52" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
@@ -4571,7 +4577,7 @@
         <v>37</v>
       </c>
       <c r="O53" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
@@ -4659,7 +4665,7 @@
         <v>133</v>
       </c>
       <c r="M55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N55" t="s">
         <v>37</v>
@@ -4759,7 +4765,7 @@
         <v>37</v>
       </c>
       <c r="O57" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -4806,7 +4812,7 @@
         <v>37</v>
       </c>
       <c r="O58" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -4853,7 +4859,7 @@
         <v>37</v>
       </c>
       <c r="O59" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
@@ -4994,7 +5000,7 @@
         <v>177</v>
       </c>
       <c r="O62" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
@@ -5041,7 +5047,7 @@
         <v>180</v>
       </c>
       <c r="O63" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
@@ -5088,7 +5094,7 @@
         <v>183</v>
       </c>
       <c r="O64" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
@@ -5114,7 +5120,7 @@
         <v>15</v>
       </c>
       <c r="H65" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I65" t="s">
         <v>17</v>
@@ -5161,7 +5167,7 @@
         <v>23</v>
       </c>
       <c r="H66" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I66" t="s">
         <v>17</v>
@@ -5208,7 +5214,7 @@
         <v>15</v>
       </c>
       <c r="H67" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I67" t="s">
         <v>17</v>
@@ -5255,7 +5261,7 @@
         <v>23</v>
       </c>
       <c r="H68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I68" t="s">
         <v>17</v>
@@ -5302,7 +5308,7 @@
         <v>23</v>
       </c>
       <c r="H69" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I69" t="s">
         <v>17</v>
@@ -5317,10 +5323,10 @@
         <v>37</v>
       </c>
       <c r="M69" t="s">
+        <v>37</v>
+      </c>
+      <c r="N69" t="s">
         <v>197</v>
-      </c>
-      <c r="N69" t="s">
-        <v>37</v>
       </c>
       <c r="O69" t="s">
         <v>37</v>
@@ -5349,7 +5355,7 @@
         <v>23</v>
       </c>
       <c r="H70" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I70" t="s">
         <v>17</v>
@@ -5411,10 +5417,10 @@
         <v>37</v>
       </c>
       <c r="M71" t="s">
+        <v>37</v>
+      </c>
+      <c r="N71" t="s">
         <v>189</v>
-      </c>
-      <c r="N71" t="s">
-        <v>37</v>
       </c>
       <c r="O71" t="s">
         <v>37</v>
@@ -5422,57 +5428,57 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B72" t="s">
-        <v>205</v>
+        <v>377</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D72" t="s">
         <v>186</v>
       </c>
       <c r="E72">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G72" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H72" t="s">
+        <v>37</v>
+      </c>
+      <c r="I72" t="s">
+        <v>17</v>
+      </c>
+      <c r="J72" t="s">
+        <v>37</v>
+      </c>
+      <c r="K72" t="s">
+        <v>37</v>
+      </c>
+      <c r="L72" t="s">
+        <v>37</v>
+      </c>
+      <c r="M72" t="s">
+        <v>37</v>
+      </c>
+      <c r="N72" t="s">
+        <v>189</v>
+      </c>
+      <c r="O72" t="s">
         <v>203</v>
-      </c>
-      <c r="I72" t="s">
-        <v>17</v>
-      </c>
-      <c r="J72" t="s">
-        <v>37</v>
-      </c>
-      <c r="K72" t="s">
-        <v>37</v>
-      </c>
-      <c r="L72" t="s">
-        <v>37</v>
-      </c>
-      <c r="M72" t="s">
-        <v>206</v>
-      </c>
-      <c r="N72" t="s">
-        <v>37</v>
-      </c>
-      <c r="O72" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B73" t="s">
-        <v>366</v>
+        <v>205</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -5484,13 +5490,13 @@
         <v>10</v>
       </c>
       <c r="F73">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H73" t="s">
-        <v>340</v>
+        <v>203</v>
       </c>
       <c r="I73" t="s">
         <v>17</v>
@@ -5505,7 +5511,7 @@
         <v>37</v>
       </c>
       <c r="M73" t="s">
-        <v>37</v>
+        <v>206</v>
       </c>
       <c r="N73" t="s">
         <v>37</v>
@@ -5516,10 +5522,10 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B74" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -5537,7 +5543,7 @@
         <v>23</v>
       </c>
       <c r="H74" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I74" t="s">
         <v>17</v>
@@ -5552,7 +5558,7 @@
         <v>37</v>
       </c>
       <c r="M74" t="s">
-        <v>209</v>
+        <v>37</v>
       </c>
       <c r="N74" t="s">
         <v>37</v>
@@ -5563,10 +5569,10 @@
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B75" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -5578,13 +5584,13 @@
         <v>10</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G75" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H75" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I75" t="s">
         <v>17</v>
@@ -5599,7 +5605,7 @@
         <v>37</v>
       </c>
       <c r="M75" t="s">
-        <v>37</v>
+        <v>209</v>
       </c>
       <c r="N75" t="s">
         <v>37</v>
@@ -5610,13 +5616,13 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B76" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
         <v>186</v>
@@ -5631,7 +5637,7 @@
         <v>15</v>
       </c>
       <c r="H76" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I76" t="s">
         <v>17</v>
@@ -5646,10 +5652,10 @@
         <v>37</v>
       </c>
       <c r="M76" t="s">
-        <v>184</v>
+        <v>37</v>
       </c>
       <c r="N76" t="s">
-        <v>219</v>
+        <v>37</v>
       </c>
       <c r="O76" t="s">
         <v>37</v>
@@ -5657,10 +5663,10 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B77" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C77">
         <v>3</v>
@@ -5678,7 +5684,7 @@
         <v>15</v>
       </c>
       <c r="H77" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I77" t="s">
         <v>17</v>
@@ -5693,10 +5699,10 @@
         <v>37</v>
       </c>
       <c r="M77" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="N77" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="O77" t="s">
         <v>37</v>
@@ -5704,10 +5710,10 @@
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B78" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -5725,7 +5731,7 @@
         <v>15</v>
       </c>
       <c r="H78" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I78" t="s">
         <v>17</v>
@@ -5740,7 +5746,7 @@
         <v>37</v>
       </c>
       <c r="M78" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
       <c r="N78" t="s">
         <v>37</v>
@@ -5751,10 +5757,10 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B79" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C79">
         <v>3</v>
@@ -5763,16 +5769,16 @@
         <v>186</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F79">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I79" t="s">
         <v>17</v>
@@ -5787,10 +5793,10 @@
         <v>37</v>
       </c>
       <c r="M79" t="s">
-        <v>347</v>
+        <v>37</v>
       </c>
       <c r="N79" t="s">
-        <v>212</v>
+        <v>37</v>
       </c>
       <c r="O79" t="s">
         <v>37</v>
@@ -5798,10 +5804,10 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B80" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -5810,16 +5816,16 @@
         <v>186</v>
       </c>
       <c r="E80">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G80" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H80" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I80" t="s">
         <v>17</v>
@@ -5834,10 +5840,10 @@
         <v>37</v>
       </c>
       <c r="M80" t="s">
-        <v>37</v>
+        <v>346</v>
       </c>
       <c r="N80" t="s">
-        <v>37</v>
+        <v>212</v>
       </c>
       <c r="O80" t="s">
         <v>37</v>
@@ -5845,10 +5851,10 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B81" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C81">
         <v>3</v>
@@ -5857,16 +5863,16 @@
         <v>186</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F81">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G81" t="s">
         <v>57</v>
       </c>
       <c r="H81" t="s">
-        <v>225</v>
+        <v>339</v>
       </c>
       <c r="I81" t="s">
         <v>17</v>
@@ -5887,15 +5893,15 @@
         <v>37</v>
       </c>
       <c r="O81" t="s">
-        <v>368</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B82" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C82">
         <v>3</v>
@@ -5907,13 +5913,13 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G82" t="s">
-        <v>23</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>362</v>
+        <v>57</v>
+      </c>
+      <c r="H82" t="s">
+        <v>225</v>
       </c>
       <c r="I82" t="s">
         <v>17</v>
@@ -5928,21 +5934,21 @@
         <v>37</v>
       </c>
       <c r="M82" t="s">
-        <v>216</v>
+        <v>37</v>
       </c>
       <c r="N82" t="s">
         <v>37</v>
       </c>
       <c r="O82" t="s">
-        <v>37</v>
+        <v>366</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B83" t="s">
-        <v>229</v>
+        <v>378</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -5960,7 +5966,7 @@
         <v>23</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I83" t="s">
         <v>17</v>
@@ -5986,10 +5992,10 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B84" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -5998,16 +6004,16 @@
         <v>186</v>
       </c>
       <c r="E84">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G84" t="s">
-        <v>15</v>
-      </c>
-      <c r="H84" t="s">
-        <v>232</v>
+        <v>23</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>362</v>
       </c>
       <c r="I84" t="s">
         <v>17</v>
@@ -6022,7 +6028,7 @@
         <v>37</v>
       </c>
       <c r="M84" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
       <c r="N84" t="s">
         <v>37</v>
@@ -6033,10 +6039,10 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B85" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -6045,16 +6051,16 @@
         <v>186</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F85">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G85" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H85" t="s">
-        <v>364</v>
+        <v>231</v>
       </c>
       <c r="I85" t="s">
         <v>17</v>
@@ -6069,21 +6075,21 @@
         <v>37</v>
       </c>
       <c r="M85" t="s">
-        <v>192</v>
+        <v>37</v>
       </c>
       <c r="N85" t="s">
         <v>37</v>
       </c>
       <c r="O85" t="s">
-        <v>367</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B86" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C86">
         <v>3</v>
@@ -6095,13 +6101,13 @@
         <v>0</v>
       </c>
       <c r="F86">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G86" t="s">
         <v>23</v>
       </c>
       <c r="H86" t="s">
-        <v>37</v>
+        <v>363</v>
       </c>
       <c r="I86" t="s">
         <v>17</v>
@@ -6116,21 +6122,21 @@
         <v>37</v>
       </c>
       <c r="M86" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="N86" t="s">
         <v>37</v>
       </c>
       <c r="O86" t="s">
-        <v>37</v>
+        <v>379</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B87" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -6163,7 +6169,7 @@
         <v>37</v>
       </c>
       <c r="M87" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
       <c r="N87" t="s">
         <v>37</v>
@@ -6174,10 +6180,10 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B88" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C88">
         <v>3</v>
@@ -6186,16 +6192,16 @@
         <v>186</v>
       </c>
       <c r="E88">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G88" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H88" t="s">
-        <v>232</v>
+        <v>37</v>
       </c>
       <c r="I88" t="s">
         <v>17</v>
@@ -6210,7 +6216,7 @@
         <v>37</v>
       </c>
       <c r="M88" t="s">
-        <v>241</v>
+        <v>37</v>
       </c>
       <c r="N88" t="s">
         <v>37</v>
@@ -6221,10 +6227,10 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B89" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C89">
         <v>3</v>
@@ -6242,7 +6248,7 @@
         <v>15</v>
       </c>
       <c r="H89" t="s">
-        <v>375</v>
+        <v>231</v>
       </c>
       <c r="I89" t="s">
         <v>17</v>
@@ -6257,21 +6263,21 @@
         <v>37</v>
       </c>
       <c r="M89" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="N89" t="s">
         <v>37</v>
       </c>
       <c r="O89" t="s">
-        <v>256</v>
+        <v>37</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B90" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C90">
         <v>3</v>
@@ -6280,16 +6286,16 @@
         <v>186</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F90">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G90" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H90" t="s">
-        <v>232</v>
+        <v>372</v>
       </c>
       <c r="I90" t="s">
         <v>17</v>
@@ -6304,21 +6310,21 @@
         <v>37</v>
       </c>
       <c r="M90" t="s">
-        <v>37</v>
+        <v>201</v>
       </c>
       <c r="N90" t="s">
         <v>37</v>
       </c>
       <c r="O90" t="s">
-        <v>37</v>
+        <v>255</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B91" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C91">
         <v>3</v>
@@ -6336,7 +6342,7 @@
         <v>23</v>
       </c>
       <c r="H91" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I91" t="s">
         <v>17</v>
@@ -6354,7 +6360,7 @@
         <v>37</v>
       </c>
       <c r="N91" t="s">
-        <v>249</v>
+        <v>37</v>
       </c>
       <c r="O91" t="s">
         <v>37</v>
@@ -6362,10 +6368,10 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B92" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C92">
         <v>3</v>
@@ -6374,16 +6380,16 @@
         <v>186</v>
       </c>
       <c r="E92">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G92" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H92" t="s">
-        <v>37</v>
+        <v>231</v>
       </c>
       <c r="I92" t="s">
         <v>17</v>
@@ -6398,21 +6404,21 @@
         <v>37</v>
       </c>
       <c r="M92" t="s">
-        <v>348</v>
+        <v>37</v>
       </c>
       <c r="N92" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="O92" t="s">
-        <v>256</v>
+        <v>37</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B93" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C93">
         <v>3</v>
@@ -6421,13 +6427,13 @@
         <v>186</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F93">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G93" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H93" t="s">
         <v>37</v>
@@ -6445,21 +6451,21 @@
         <v>37</v>
       </c>
       <c r="M93" t="s">
-        <v>216</v>
+        <v>347</v>
       </c>
       <c r="N93" t="s">
-        <v>37</v>
+        <v>241</v>
       </c>
       <c r="O93" t="s">
-        <v>37</v>
+        <v>255</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B94" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C94">
         <v>3</v>
@@ -6468,16 +6474,16 @@
         <v>186</v>
       </c>
       <c r="E94">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G94" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H94" t="s">
-        <v>256</v>
+        <v>37</v>
       </c>
       <c r="I94" t="s">
         <v>17</v>
@@ -6492,24 +6498,24 @@
         <v>37</v>
       </c>
       <c r="M94" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
       <c r="N94" t="s">
         <v>37</v>
       </c>
       <c r="O94" t="s">
-        <v>369</v>
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B95" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D95" t="s">
         <v>186</v>
@@ -6518,13 +6524,13 @@
         <v>10</v>
       </c>
       <c r="F95">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G95" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="H95" t="s">
-        <v>377</v>
+        <v>255</v>
       </c>
       <c r="I95" t="s">
         <v>17</v>
@@ -6545,15 +6551,15 @@
         <v>37</v>
       </c>
       <c r="O95" t="s">
-        <v>37</v>
+        <v>380</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B96" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C96">
         <v>4</v>
@@ -6571,7 +6577,7 @@
         <v>23</v>
       </c>
       <c r="H96" t="s">
-        <v>262</v>
+        <v>374</v>
       </c>
       <c r="I96" t="s">
         <v>17</v>
@@ -6586,7 +6592,7 @@
         <v>37</v>
       </c>
       <c r="M96" t="s">
-        <v>263</v>
+        <v>37</v>
       </c>
       <c r="N96" t="s">
         <v>37</v>
@@ -6597,10 +6603,10 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B97" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C97">
         <v>4</v>
@@ -6618,7 +6624,7 @@
         <v>23</v>
       </c>
       <c r="H97" t="s">
-        <v>378</v>
+        <v>261</v>
       </c>
       <c r="I97" t="s">
         <v>17</v>
@@ -6633,7 +6639,7 @@
         <v>37</v>
       </c>
       <c r="M97" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="N97" t="s">
         <v>37</v>
@@ -6644,10 +6650,10 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B98" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C98">
         <v>4</v>
@@ -6665,7 +6671,7 @@
         <v>23</v>
       </c>
       <c r="H98" t="s">
-        <v>259</v>
+        <v>375</v>
       </c>
       <c r="I98" t="s">
         <v>17</v>
@@ -6680,21 +6686,21 @@
         <v>37</v>
       </c>
       <c r="M98" t="s">
-        <v>37</v>
+        <v>265</v>
       </c>
       <c r="N98" t="s">
         <v>37</v>
       </c>
       <c r="O98" t="s">
-        <v>273</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B99" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C99">
         <v>4</v>
@@ -6703,16 +6709,16 @@
         <v>186</v>
       </c>
       <c r="E99">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F99">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G99" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H99" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I99" t="s">
         <v>17</v>
@@ -6733,15 +6739,15 @@
         <v>37</v>
       </c>
       <c r="O99" t="s">
-        <v>370</v>
+        <v>272</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B100" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C100">
         <v>4</v>
@@ -6750,16 +6756,16 @@
         <v>186</v>
       </c>
       <c r="E100">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F100">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G100" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="H100" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="I100" t="s">
         <v>17</v>
@@ -6774,21 +6780,21 @@
         <v>37</v>
       </c>
       <c r="M100" t="s">
-        <v>274</v>
+        <v>37</v>
       </c>
       <c r="N100" t="s">
         <v>37</v>
       </c>
       <c r="O100" t="s">
-        <v>37</v>
+        <v>367</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B101" t="s">
-        <v>374</v>
+        <v>271</v>
       </c>
       <c r="C101">
         <v>4</v>
@@ -6797,16 +6803,16 @@
         <v>186</v>
       </c>
       <c r="E101">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F101">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G101" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H101" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="I101" t="s">
         <v>17</v>
@@ -6821,21 +6827,21 @@
         <v>37</v>
       </c>
       <c r="M101" t="s">
-        <v>37</v>
+        <v>273</v>
       </c>
       <c r="N101" t="s">
         <v>37</v>
       </c>
       <c r="O101" t="s">
-        <v>273</v>
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B102" t="s">
-        <v>277</v>
+        <v>371</v>
       </c>
       <c r="C102">
         <v>4</v>
@@ -6844,16 +6850,16 @@
         <v>186</v>
       </c>
       <c r="E102">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G102" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="H102" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="I102" t="s">
         <v>17</v>
@@ -6868,21 +6874,21 @@
         <v>37</v>
       </c>
       <c r="M102" t="s">
-        <v>278</v>
+        <v>37</v>
       </c>
       <c r="N102" t="s">
         <v>37</v>
       </c>
       <c r="O102" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B103" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C103">
         <v>4</v>
@@ -6891,16 +6897,16 @@
         <v>186</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F103">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G103" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H103" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I103" t="s">
         <v>17</v>
@@ -6915,21 +6921,21 @@
         <v>37</v>
       </c>
       <c r="M103" t="s">
-        <v>230</v>
+        <v>277</v>
       </c>
       <c r="N103" t="s">
         <v>37</v>
       </c>
       <c r="O103" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B104" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C104">
         <v>4</v>
@@ -6938,16 +6944,16 @@
         <v>186</v>
       </c>
       <c r="E104">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F104">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G104" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H104" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I104" t="s">
         <v>17</v>
@@ -6962,39 +6968,39 @@
         <v>37</v>
       </c>
       <c r="M104" t="s">
-        <v>37</v>
+        <v>229</v>
       </c>
       <c r="N104" t="s">
         <v>37</v>
       </c>
       <c r="O104" t="s">
-        <v>37</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B105" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C105">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D105" t="s">
-        <v>285</v>
+        <v>186</v>
       </c>
       <c r="E105">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F105">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G105" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="H105" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="I105" t="s">
         <v>17</v>
@@ -7020,16 +7026,16 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B106" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E106">
         <v>15</v>
@@ -7041,7 +7047,7 @@
         <v>23</v>
       </c>
       <c r="H106" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I106" t="s">
         <v>17</v>
@@ -7067,28 +7073,28 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B107" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C107">
         <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E107">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F107">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G107" t="s">
         <v>23</v>
       </c>
       <c r="H107" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I107" t="s">
         <v>17</v>
@@ -7114,28 +7120,28 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B108" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C108">
         <v>2</v>
       </c>
       <c r="D108" t="s">
+        <v>290</v>
+      </c>
+      <c r="E108">
+        <v>10</v>
+      </c>
+      <c r="F108">
+        <v>10</v>
+      </c>
+      <c r="G108" t="s">
+        <v>23</v>
+      </c>
+      <c r="H108" t="s">
         <v>291</v>
-      </c>
-      <c r="E108">
-        <v>10</v>
-      </c>
-      <c r="F108">
-        <v>10</v>
-      </c>
-      <c r="G108" t="s">
-        <v>295</v>
-      </c>
-      <c r="H108" t="s">
-        <v>292</v>
       </c>
       <c r="I108" t="s">
         <v>17</v>
@@ -7161,28 +7167,28 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B109" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
       <c r="D109" t="s">
+        <v>290</v>
+      </c>
+      <c r="E109">
+        <v>10</v>
+      </c>
+      <c r="F109">
+        <v>10</v>
+      </c>
+      <c r="G109" t="s">
+        <v>294</v>
+      </c>
+      <c r="H109" t="s">
         <v>291</v>
-      </c>
-      <c r="E109">
-        <v>10</v>
-      </c>
-      <c r="F109">
-        <v>10</v>
-      </c>
-      <c r="G109" t="s">
-        <v>57</v>
-      </c>
-      <c r="H109" t="s">
-        <v>352</v>
       </c>
       <c r="I109" t="s">
         <v>17</v>
@@ -7208,16 +7214,16 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B110" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C110">
         <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E110">
         <v>10</v>
@@ -7226,16 +7232,16 @@
         <v>10</v>
       </c>
       <c r="G110" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="H110" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I110" t="s">
         <v>17</v>
       </c>
       <c r="J110" t="s">
-        <v>301</v>
+        <v>37</v>
       </c>
       <c r="K110" t="s">
         <v>37</v>
@@ -7255,16 +7261,16 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B111" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C111">
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="E111">
         <v>10</v>
@@ -7273,16 +7279,16 @@
         <v>10</v>
       </c>
       <c r="G111" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H111" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="I111" t="s">
         <v>17</v>
       </c>
       <c r="J111" t="s">
-        <v>37</v>
+        <v>300</v>
       </c>
       <c r="K111" t="s">
         <v>37</v>
@@ -7291,7 +7297,7 @@
         <v>37</v>
       </c>
       <c r="M111" t="s">
-        <v>299</v>
+        <v>37</v>
       </c>
       <c r="N111" t="s">
         <v>37</v>
@@ -7302,75 +7308,75 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>301</v>
+      </c>
+      <c r="B112" t="s">
+        <v>302</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+      <c r="D112" t="s">
+        <v>303</v>
+      </c>
+      <c r="E112">
+        <v>10</v>
+      </c>
+      <c r="F112">
+        <v>10</v>
+      </c>
+      <c r="G112" t="s">
+        <v>57</v>
+      </c>
+      <c r="H112" t="s">
+        <v>325</v>
+      </c>
+      <c r="I112" t="s">
+        <v>17</v>
+      </c>
+      <c r="J112" t="s">
+        <v>37</v>
+      </c>
+      <c r="K112" t="s">
+        <v>37</v>
+      </c>
+      <c r="L112" t="s">
+        <v>37</v>
+      </c>
+      <c r="M112" t="s">
+        <v>298</v>
+      </c>
+      <c r="N112" t="s">
+        <v>37</v>
+      </c>
+      <c r="O112" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>304</v>
+      </c>
+      <c r="B113" t="s">
         <v>305</v>
-      </c>
-      <c r="B112" t="s">
-        <v>306</v>
-      </c>
-      <c r="C112">
-        <v>3</v>
-      </c>
-      <c r="D112" t="s">
-        <v>285</v>
-      </c>
-      <c r="E112">
-        <v>10</v>
-      </c>
-      <c r="F112">
-        <v>10</v>
-      </c>
-      <c r="G112" t="s">
-        <v>23</v>
-      </c>
-      <c r="H112" t="s">
-        <v>286</v>
-      </c>
-      <c r="I112" t="s">
-        <v>17</v>
-      </c>
-      <c r="J112" t="s">
-        <v>37</v>
-      </c>
-      <c r="K112" t="s">
-        <v>37</v>
-      </c>
-      <c r="L112" t="s">
-        <v>37</v>
-      </c>
-      <c r="M112" t="s">
-        <v>37</v>
-      </c>
-      <c r="N112" t="s">
-        <v>37</v>
-      </c>
-      <c r="O112" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>308</v>
       </c>
       <c r="C113">
         <v>3</v>
       </c>
       <c r="D113" t="s">
+        <v>284</v>
+      </c>
+      <c r="E113">
+        <v>10</v>
+      </c>
+      <c r="F113">
+        <v>10</v>
+      </c>
+      <c r="G113" t="s">
+        <v>23</v>
+      </c>
+      <c r="H113" t="s">
         <v>285</v>
-      </c>
-      <c r="E113">
-        <v>10</v>
-      </c>
-      <c r="F113">
-        <v>10</v>
-      </c>
-      <c r="G113" t="s">
-        <v>295</v>
-      </c>
-      <c r="H113" t="s">
-        <v>37</v>
       </c>
       <c r="I113" t="s">
         <v>17</v>
@@ -7396,16 +7402,16 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C114">
         <v>3</v>
       </c>
       <c r="D114" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E114">
         <v>10</v>
@@ -7414,7 +7420,7 @@
         <v>10</v>
       </c>
       <c r="G114" t="s">
-        <v>23</v>
+        <v>294</v>
       </c>
       <c r="H114" t="s">
         <v>37</v>
@@ -7443,25 +7449,25 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C115">
         <v>3</v>
       </c>
       <c r="D115" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E115">
         <v>10</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G115" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H115" t="s">
         <v>37</v>
@@ -7490,25 +7496,25 @@
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C116">
         <v>3</v>
       </c>
       <c r="D116" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F116">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G116" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="H116" t="s">
         <v>37</v>
@@ -7537,16 +7543,16 @@
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C117">
         <v>3</v>
       </c>
       <c r="D117" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -7584,19 +7590,19 @@
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="B118" t="s">
-        <v>318</v>
+        <v>314</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>315</v>
       </c>
       <c r="C118">
         <v>3</v>
       </c>
       <c r="D118" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E118">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F118">
         <v>10</v>
@@ -7605,7 +7611,7 @@
         <v>23</v>
       </c>
       <c r="H118" t="s">
-        <v>292</v>
+        <v>37</v>
       </c>
       <c r="I118" t="s">
         <v>17</v>
@@ -7631,16 +7637,16 @@
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B119" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C119">
         <v>3</v>
       </c>
       <c r="D119" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E119">
         <v>10</v>
@@ -7652,7 +7658,7 @@
         <v>23</v>
       </c>
       <c r="H119" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I119" t="s">
         <v>17</v>
@@ -7678,16 +7684,16 @@
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
+      </c>
+      <c r="B120" t="s">
+        <v>319</v>
       </c>
       <c r="C120">
         <v>3</v>
       </c>
       <c r="D120" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E120">
         <v>10</v>
@@ -7699,7 +7705,7 @@
         <v>23</v>
       </c>
       <c r="H120" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="I120" t="s">
         <v>17</v>
@@ -7725,16 +7731,16 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C121">
         <v>3</v>
       </c>
       <c r="D121" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E121">
         <v>10</v>
@@ -7746,7 +7752,7 @@
         <v>23</v>
       </c>
       <c r="H121" t="s">
-        <v>118</v>
+        <v>297</v>
       </c>
       <c r="I121" t="s">
         <v>17</v>
@@ -7761,7 +7767,7 @@
         <v>37</v>
       </c>
       <c r="M121" t="s">
-        <v>299</v>
+        <v>37</v>
       </c>
       <c r="N121" t="s">
         <v>37</v>
@@ -7772,16 +7778,16 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B122" t="s">
-        <v>325</v>
+        <v>300</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>322</v>
       </c>
       <c r="C122">
         <v>3</v>
       </c>
       <c r="D122" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="E122">
         <v>10</v>
@@ -7790,10 +7796,10 @@
         <v>10</v>
       </c>
       <c r="G122" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H122" t="s">
-        <v>326</v>
+        <v>118</v>
       </c>
       <c r="I122" t="s">
         <v>17</v>
@@ -7808,7 +7814,7 @@
         <v>37</v>
       </c>
       <c r="M122" t="s">
-        <v>37</v>
+        <v>298</v>
       </c>
       <c r="N122" t="s">
         <v>37</v>
@@ -7818,17 +7824,17 @@
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>327</v>
+      <c r="A123" s="3" t="s">
+        <v>323</v>
       </c>
       <c r="B123" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C123">
         <v>3</v>
       </c>
       <c r="D123" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
       <c r="E123">
         <v>10</v>
@@ -7840,7 +7846,7 @@
         <v>57</v>
       </c>
       <c r="H123" t="s">
-        <v>37</v>
+        <v>325</v>
       </c>
       <c r="I123" t="s">
         <v>17</v>
@@ -7865,53 +7871,103 @@
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
-        <v>360</v>
+      <c r="A124" t="s">
+        <v>326</v>
       </c>
       <c r="B124" t="s">
-        <v>361</v>
+        <v>327</v>
       </c>
       <c r="C124">
         <v>3</v>
       </c>
       <c r="D124" t="s">
+        <v>328</v>
+      </c>
+      <c r="E124">
+        <v>10</v>
+      </c>
+      <c r="F124">
+        <v>10</v>
+      </c>
+      <c r="G124" t="s">
+        <v>57</v>
+      </c>
+      <c r="H124" t="s">
+        <v>37</v>
+      </c>
+      <c r="I124" t="s">
+        <v>17</v>
+      </c>
+      <c r="J124" t="s">
+        <v>37</v>
+      </c>
+      <c r="K124" t="s">
+        <v>37</v>
+      </c>
+      <c r="L124" t="s">
+        <v>37</v>
+      </c>
+      <c r="M124" t="s">
+        <v>37</v>
+      </c>
+      <c r="N124" t="s">
+        <v>37</v>
+      </c>
+      <c r="O124" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B125" t="s">
+        <v>360</v>
+      </c>
+      <c r="C125">
+        <v>3</v>
+      </c>
+      <c r="D125" t="s">
         <v>186</v>
       </c>
-      <c r="E124">
-        <v>10</v>
-      </c>
-      <c r="F124">
-        <v>0</v>
-      </c>
-      <c r="G124" t="s">
+      <c r="E125">
+        <v>10</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125" t="s">
         <v>15</v>
       </c>
-      <c r="I124" t="s">
-        <v>17</v>
-      </c>
-      <c r="J124" t="s">
-        <v>37</v>
-      </c>
-      <c r="K124" t="s">
-        <v>37</v>
-      </c>
-      <c r="L124" t="s">
-        <v>37</v>
-      </c>
-      <c r="M124" t="s">
-        <v>37</v>
-      </c>
-      <c r="N124" t="s">
-        <v>37</v>
-      </c>
-      <c r="O124" t="s">
+      <c r="H125" t="s">
+        <v>37</v>
+      </c>
+      <c r="I125" t="s">
+        <v>17</v>
+      </c>
+      <c r="J125" t="s">
+        <v>37</v>
+      </c>
+      <c r="K125" t="s">
+        <v>37</v>
+      </c>
+      <c r="L125" t="s">
+        <v>37</v>
+      </c>
+      <c r="M125" t="s">
+        <v>37</v>
+      </c>
+      <c r="N125" t="s">
+        <v>37</v>
+      </c>
+      <c r="O125" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K124" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K104">
-      <sortCondition ref="A1:A104"/>
+  <autoFilter ref="A1:K125" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K105">
+      <sortCondition ref="A1:A105"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="21" type="noConversion"/>

</xml_diff>

<commit_message>
Fix bugs with MAS8707
</commit_message>
<xml_diff>
--- a/Modules.xlsx
+++ b/Modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joematthews/Desktop/PreReg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9960C115-F77D-AB49-88C6-07DF664F52BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A37D60-7F14-A84B-B598-4F09516F9B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Working App back end " sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="382">
   <si>
     <t>Code</t>
   </si>
@@ -1181,6 +1181,9 @@
   </si>
   <si>
     <t>F3F5;F3FM;F344;F345</t>
+  </si>
+  <si>
+    <t>GL11;NG41</t>
   </si>
 </sst>
 </file>
@@ -2066,10 +2069,10 @@
   <dimension ref="A1:O125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O96" sqref="O96"/>
+      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3355,7 +3358,7 @@
         <v>82</v>
       </c>
       <c r="O27" t="s">
-        <v>37</v>
+        <v>381</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -4218,10 +4221,10 @@
         <v>14</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F46">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G46" t="s">
         <v>23</v>
@@ -5464,10 +5467,10 @@
         <v>37</v>
       </c>
       <c r="M72" t="s">
-        <v>37</v>
+        <v>189</v>
       </c>
       <c r="N72" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
       <c r="O72" t="s">
         <v>203</v>

</xml_diff>

<commit_message>
Fix JH bugs, simplified spreadsheet to focus on standard JH comp codes
</commit_message>
<xml_diff>
--- a/Modules.xlsx
+++ b/Modules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joematthews/Desktop/PreReg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A37D60-7F14-A84B-B598-4F09516F9B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE84215-7315-C147-9DC4-28F5FDFFAB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Working App back end " sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="379">
   <si>
     <t>Code</t>
   </si>
@@ -1099,24 +1099,6 @@
     <t>G1N3;ACC2</t>
   </si>
   <si>
-    <t>PJH;MWFSP;MWBJP</t>
-  </si>
-  <si>
-    <t>PJH;P2JH;MWFSP;MWFSB;MWBJP;MWBPA;MWBPS</t>
-  </si>
-  <si>
-    <t>AJH;A2JH;MWFSA;MWFSB;MWBJA;MWBPA;MWBAS</t>
-  </si>
-  <si>
-    <t>AJH;MWFSA;MWBJA</t>
-  </si>
-  <si>
-    <t>SJH;S2JH;G1N3;MWBJS;MWBPS;MWBAS</t>
-  </si>
-  <si>
-    <t>SJH;MWBJS</t>
-  </si>
-  <si>
     <t>CEG3707</t>
   </si>
   <si>
@@ -1159,9 +1141,6 @@
     <t>F344;F345</t>
   </si>
   <si>
-    <t>PJH;P2JH;MWFSP;MWFSB;MWPJP;MWBPA;MWBPS;MWBJP</t>
-  </si>
-  <si>
     <t>F303;MPWA1</t>
   </si>
   <si>
@@ -1184,6 +1163,18 @@
   </si>
   <si>
     <t>GL11;NG41</t>
+  </si>
+  <si>
+    <t>AJH;A2JH;MWFSB;MWBPA;MWBAS</t>
+  </si>
+  <si>
+    <t>AJH;A2JH;MWFSB;;MWBPA;MWBAS</t>
+  </si>
+  <si>
+    <t>SJH;S2JH;G1N3;MWBPS;MWBAS</t>
+  </si>
+  <si>
+    <t>PJH;P2JH;MWFSB;MWBPA;MWBPS</t>
   </si>
 </sst>
 </file>
@@ -2069,10 +2060,10 @@
   <dimension ref="A1:O125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2136,7 +2127,7 @@
         <v>349</v>
       </c>
       <c r="O1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -2162,7 +2153,7 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>354</v>
+        <v>378</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -2209,7 +2200,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>353</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -2256,7 +2247,7 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>353</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
@@ -2303,7 +2294,7 @@
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -2350,7 +2341,7 @@
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
@@ -2397,7 +2388,7 @@
         <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
@@ -2444,7 +2435,7 @@
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
@@ -2491,7 +2482,7 @@
         <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
@@ -2538,7 +2529,7 @@
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -2585,7 +2576,7 @@
         <v>23</v>
       </c>
       <c r="H11" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="I11" t="s">
         <v>17</v>
@@ -2632,7 +2623,7 @@
         <v>23</v>
       </c>
       <c r="H12" t="s">
-        <v>358</v>
+        <v>43</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
@@ -2679,7 +2670,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>358</v>
+        <v>43</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
@@ -3358,7 +3349,7 @@
         <v>82</v>
       </c>
       <c r="O27" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -3572,7 +3563,7 @@
         <v>23</v>
       </c>
       <c r="H32" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="I32" t="s">
         <v>17</v>
@@ -3854,7 +3845,7 @@
         <v>15</v>
       </c>
       <c r="H38" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="I38" t="s">
         <v>17</v>
@@ -3948,7 +3939,7 @@
         <v>57</v>
       </c>
       <c r="H40" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="I40" t="s">
         <v>17</v>
@@ -4439,7 +4430,7 @@
         <v>37</v>
       </c>
       <c r="O50" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -4486,7 +4477,7 @@
         <v>37</v>
       </c>
       <c r="O51" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -4533,7 +4524,7 @@
         <v>37</v>
       </c>
       <c r="O52" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
@@ -4580,7 +4571,7 @@
         <v>37</v>
       </c>
       <c r="O53" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
@@ -4768,7 +4759,7 @@
         <v>37</v>
       </c>
       <c r="O57" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -4815,7 +4806,7 @@
         <v>37</v>
       </c>
       <c r="O58" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -4862,7 +4853,7 @@
         <v>37</v>
       </c>
       <c r="O59" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
@@ -5003,7 +4994,7 @@
         <v>177</v>
       </c>
       <c r="O62" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
@@ -5050,7 +5041,7 @@
         <v>180</v>
       </c>
       <c r="O63" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
@@ -5097,7 +5088,7 @@
         <v>183</v>
       </c>
       <c r="O64" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
@@ -5434,7 +5425,7 @@
         <v>201</v>
       </c>
       <c r="B72" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="C72">
         <v>3</v>
@@ -5528,7 +5519,7 @@
         <v>197</v>
       </c>
       <c r="B74" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -5943,7 +5934,7 @@
         <v>37</v>
       </c>
       <c r="O82" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
@@ -5951,7 +5942,7 @@
         <v>226</v>
       </c>
       <c r="B83" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -5969,7 +5960,7 @@
         <v>23</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="I83" t="s">
         <v>17</v>
@@ -6016,7 +6007,7 @@
         <v>23</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="I84" t="s">
         <v>17</v>
@@ -6110,7 +6101,7 @@
         <v>23</v>
       </c>
       <c r="H86" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="I86" t="s">
         <v>17</v>
@@ -6131,7 +6122,7 @@
         <v>37</v>
       </c>
       <c r="O86" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
@@ -6298,7 +6289,7 @@
         <v>15</v>
       </c>
       <c r="H90" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="I90" t="s">
         <v>17</v>
@@ -6554,7 +6545,7 @@
         <v>37</v>
       </c>
       <c r="O95" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
@@ -6580,7 +6571,7 @@
         <v>23</v>
       </c>
       <c r="H96" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="I96" t="s">
         <v>17</v>
@@ -6674,7 +6665,7 @@
         <v>23</v>
       </c>
       <c r="H98" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="I98" t="s">
         <v>17</v>
@@ -6789,7 +6780,7 @@
         <v>37</v>
       </c>
       <c r="O100" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.2">
@@ -6844,7 +6835,7 @@
         <v>274</v>
       </c>
       <c r="B102" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C102">
         <v>4</v>
@@ -7922,10 +7913,10 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B125" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C125">
         <v>3</v>

</xml_diff>